<commit_message>
Updated scripts to read multiple release versions
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs002431_Gender_Female.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs002431_Gender_Female.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-06-21-2024/Commons_Automation/InputFiles/CDS/phs002431/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714D0E39-0172-9841-A94C-5B6913B574C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6776E74-1C9F-3F40-80A9-ACEC4124BAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40400" yWindow="2700" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -61,45 +61,6 @@
   </si>
   <si>
     <t>TC01_CDS_phs002431_Gender_Female_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT
-    f1.file_name AS "File Name",
-    s.study_name AS "Study Name",
-    s.phs_accession AS "Accession",
-    sp.participant_id AS "Participant Id",
-    COALESCE((
-        SELECT
-            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
-            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
-        FROM (
-            SELECT
-                smp.sample_id,
-                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
-            FROM df_sample smp
-            WHERE smp."participant.study_participant_id" = sp.study_participant_id
-        ) smp
-    ), '') AS "Sample Id",
-    f1.file_type AS "File Type"
-FROM 
-    df_study s
-INNER JOIN 
-    df_participant sp ON sp."study.phs_accession" = s.phs_accession
-INNER JOIN  
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN 
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-WHERE 
-    s.phs_accession = 'phs002431' AND sp.gender = 'Female'
-GROUP BY
-    f1.file_name,
-    s.study_name,
-    s.phs_accession,
-    sp.participant_id,
-    f1.file_type
-ORDER BY 
-    f1.file_name ASC
-LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT
@@ -126,7 +87,7 @@
 ON
     f."sample.sample_id" = smp.sample_id
 WHERE 
-    s.phs_accession='phs002431' AND sp.gender = 'Female'</t>
+   s.phs_accession = 'phs004231' AND sp.gender = 'Female'</t>
   </si>
   <si>
     <t>WITH Distinct_Samples AS (
@@ -148,7 +109,7 @@
     ON 
         smp."participant.study_participant_id" = sp.study_participant_id
     WHERE 
-        s.phs_accession = 'phs002431' AND sp.gender = 'Female'
+        s.phs_accession = 'phs004231' AND sp.gender = 'Female'
 ),
 Sample_Limit AS (
     SELECT
@@ -186,7 +147,7 @@
 LIMIT 100;</t>
   </si>
   <si>
-    <t>SELECT
+    <t xml:space="preserve">SELECT
     DISTINCT (smp.sample_id) AS "Sample ID",
     sp.participant_id AS "Participant ID", 
     s.study_name AS "Study Name",
@@ -204,26 +165,57 @@
 ON 
     smp."participant.study_participant_id" = sp.study_participant_id
 WHERE 
-    s.phs_accession = 'phs002431' AND sp.gender = 'Female'
+    s.phs_accession = 'phs004231' AND sp.gender = 'Female'
 ORDER BY 
     smp.sample_id  ASC
-LIMIT 100</t>
+</t>
+  </si>
+  <si>
+    <t>SELECT
+    f1.file_name AS "File Name",
+    s.study_name AS "Study Name",
+    s.phs_accession AS "Accession",
+    sp.participant_id AS "Participant Id",
+    COALESCE((
+        SELECT
+            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
+            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
+        FROM (
+            SELECT
+                smp.sample_id,
+                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
+            FROM df_sample smp
+            WHERE smp."participant.study_participant_id" = sp.study_participant_id
+        ) smp
+    ), '') AS "Sample Id",
+    f1.file_type AS "File Type"
+FROM 
+    df_study s
+INNER JOIN 
+    df_participant sp ON sp."study.phs_accession" = s.phs_accession
+INNER JOIN  
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN 
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+WHERE 
+    s.phs_accession = 'phs004231' AND sp.gender = 'Female'
+GROUP BY
+    f1.file_name,
+    s.study_name,
+    s.phs_accession,
+    sp.participant_id,
+    f1.file_type
+ORDER BY 
+    f1.file_name ASC;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -276,17 +268,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,7 +599,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -642,11 +631,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -659,8 +648,8 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -669,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -681,7 +670,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>